<commit_message>
Estimation page modified 07-02-2023
</commit_message>
<xml_diff>
--- a/JewellPro/template/Estimation.xlsx
+++ b/JewellPro/template/Estimation.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>ESTIMATION</t>
   </si>
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Date : </t>
   </si>
   <si>
-    <t>GOLD SMITH JEWELLERY</t>
+    <t>APS JEWELLERY</t>
   </si>
   <si>
     <t>75-A1, Thiru Nagar, 
@@ -47,8 +47,7 @@
     <t>Purity</t>
   </si>
   <si>
-    <t>Approximate Wt 
-(in grams)</t>
+    <t>Approximate Wt  (in grams)</t>
   </si>
   <si>
     <t>Gold 
@@ -77,31 +76,23 @@
 Standard Chartered Bank | Account Name: Arun Prakash. B | Account No: 43510215496 | Branch: Coimbatore Branch | IFSC Code: SCBL0036077
 Google Pay: +91 9894178820.</t>
   </si>
-  <si>
-    <t xml:space="preserve">Standard Gold Rate: 22 Karat (91.6% Purity) – Rs. 4,885/- | Gold Rate: (85% Purity) – Rs. 4,530/- Gold </t>
-  </si>
-  <si>
-    <t>Rate Frozen: No | Frozen Date: Nil | Customer Signature: Nil</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -109,7 +100,23 @@
       <sz val="15"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF9900"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,43 +124,354 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <color rgb="FFFF9900"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -174,11 +492,264 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -186,86 +757,135 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFFF9900"/>
+      <color rgb="00FF9900"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -548,141 +1168,147 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:H4"/>
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.1" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.74074074074074" customWidth="1"/>
+    <col min="2" max="2" width="17.037037037037" customWidth="1"/>
+    <col min="3" max="3" width="7.22222222222222" customWidth="1"/>
+    <col min="4" max="4" width="8.88888888888889" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.0740740740741" customWidth="1"/>
+    <col min="7" max="7" width="11.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="17.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="22" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:8">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="23"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" s="1" customFormat="1" ht="30" customHeight="1" spans="1:8">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-    </row>
-    <row r="4" spans="1:8" ht="90.75" customHeight="1">
-      <c r="A4" s="19" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" ht="90.75" customHeight="1" spans="1:8">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" ht="19.5" customHeight="1" spans="1:8">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1">
-      <c r="A6" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1">
-      <c r="A7" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+    </row>
+    <row r="6" ht="30" customHeight="1" spans="1:8">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+    </row>
+    <row r="7" ht="30" customHeight="1" spans="1:8">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="48" customHeight="1" spans="1:8">
+      <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E8" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H8" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1">
+    <row r="9" ht="39.95" customHeight="1" spans="1:8">
+      <c r="A9" s="2"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="22"/>
+    </row>
+    <row r="10" ht="39.95" customHeight="1" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -690,9 +1316,9 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="H10" s="22"/>
+    </row>
+    <row r="11" ht="39.95" customHeight="1" spans="1:8">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -700,9 +1326,9 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="H11" s="22"/>
+    </row>
+    <row r="12" ht="39.95" customHeight="1" spans="1:8">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -710,9 +1336,9 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="H12" s="22"/>
+    </row>
+    <row r="13" ht="39.95" customHeight="1" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -720,9 +1346,9 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" ht="39.95" customHeight="1" spans="1:8">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -730,9 +1356,9 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1">
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" ht="39.95" customHeight="1" spans="1:8">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -740,63 +1366,48 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" s="1" customFormat="1" customHeight="1" spans="1:8">
+      <c r="A16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3" t="s">
+      <c r="E16" s="19"/>
+      <c r="F16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="120" customHeight="1">
-      <c r="A19" s="12" t="s">
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="18" s="3" customFormat="1" ht="120" customHeight="1" spans="1:1">
+      <c r="A18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="F2:G2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="E3:H3"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:H4"/>
-    <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:H5"/>
     <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="E5:H5"/>
     <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="A18:H18"/>
   </mergeCells>
-  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.54166666666666663" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.118110236220472" right="0.118110236220472" top="0.541666666666667" bottom="0.748031496062992" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"-,Bold"&amp;KFF0000100 BIS HALLMARKED | TRANSPARENT PRICE BREAKUP | LIFETIME EXCHANGE | LIFETIME BUY BACK&amp;K01+000
 G O L D S M I T H JEWELLERY – SINCE 1975 | WE CRAFT YOUR FAVORITE JEWELS&amp;"-,Regular"

</xml_diff>